<commit_message>
Updated GBDS File | September 2025
</commit_message>
<xml_diff>
--- a/GBDS SEPTEMBER FILES 2025/Credits.xlsx
+++ b/GBDS SEPTEMBER FILES 2025/Credits.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GBDS AUGUST FILES 2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GBDS SEPTEMBER FILES 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999F71F0-A740-4D56-ABA8-A67FA494154D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C188E59C-AA58-4383-BEA3-6D365FBB0856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5E8FA85-F4A4-49C3-B22A-2EB131040871}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$H$12:$M$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>LESS: CREDIT</t>
   </si>
@@ -90,15 +90,6 @@
     <t>ELSIE EMBOR</t>
   </si>
   <si>
-    <t>08/20/2025</t>
-  </si>
-  <si>
-    <t>JMCC STORE</t>
-  </si>
-  <si>
-    <t>JANNA SIMBLANTE</t>
-  </si>
-  <si>
     <t>ALEJANDRO PIZON</t>
   </si>
   <si>
@@ -109,6 +100,12 @@
   </si>
   <si>
     <t>08/29/2025</t>
+  </si>
+  <si>
+    <t>AIRA TENG</t>
+  </si>
+  <si>
+    <t>ARACELIE ALESNA</t>
   </si>
 </sst>
 </file>
@@ -415,17 +412,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -436,10 +434,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -456,28 +475,6 @@
     </xf>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,7 +792,7 @@
   <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,26 +804,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="28"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="29"/>
       <c r="F1" s="4"/>
       <c r="G1" s="8"/>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="27" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="28"/>
+      <c r="L1" s="29"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
@@ -843,11 +840,11 @@
       <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="36"/>
       <c r="G2" s="8"/>
       <c r="H2" s="13" t="s">
         <v>12</v>
@@ -855,11 +852,11 @@
       <c r="I2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="31"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="4"/>
       <c r="N2" s="8"/>
       <c r="T2" s="8"/>
@@ -871,134 +868,134 @@
       <c r="B3" s="1">
         <v>5603</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="18">
         <v>84657</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
       <c r="H3" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I3" s="16">
         <v>4320</v>
       </c>
-      <c r="J3" s="32">
+      <c r="J3" s="40">
         <v>3925</v>
       </c>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
     </row>
     <row r="4" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2">
         <v>5606</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="19">
         <v>18260</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
       <c r="H4" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I4" s="17">
         <v>4319</v>
       </c>
-      <c r="J4" s="33">
+      <c r="J4" s="41">
         <v>2355</v>
       </c>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
     </row>
     <row r="5" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
       <c r="H5" s="15"/>
       <c r="I5" s="17"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
     </row>
     <row r="6" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
       <c r="H6" s="15"/>
       <c r="I6" s="17"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
       <c r="H7" s="3"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
     </row>
     <row r="8" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
     </row>
     <row r="9" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
     </row>
     <row r="10" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
       <c r="H10" s="6"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
     </row>
     <row r="11" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="22">
         <f>SUM(C3:C10)</f>
         <v>102917</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="21"/>
+      <c r="I11" s="24"/>
       <c r="J11" s="22">
         <f>SUM(J3:J10)</f>
         <v>6280</v>
@@ -1010,25 +1007,25 @@
       <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="38" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="28"/>
+      <c r="E13" s="29"/>
       <c r="F13" s="4"/>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="25"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="L13" s="28"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="30">
+        <v>45817</v>
+      </c>
+      <c r="L13" s="29"/>
     </row>
     <row r="14" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -1037,22 +1034,22 @@
       <c r="B14" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="37"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
       <c r="H14" s="13" t="s">
         <v>12</v>
       </c>
       <c r="I14" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="K14" s="30"/>
-      <c r="L14" s="31"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="39"/>
     </row>
     <row r="15" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -1061,22 +1058,22 @@
       <c r="B15" s="1">
         <v>4487</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="18">
         <v>674</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
       <c r="H15" s="15" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I15" s="16">
-        <v>5267</v>
-      </c>
-      <c r="J15" s="32">
-        <v>119937</v>
-      </c>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
+        <v>4141</v>
+      </c>
+      <c r="J15" s="40">
+        <v>1348</v>
+      </c>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
     </row>
     <row r="16" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -1085,22 +1082,22 @@
       <c r="B16" s="2">
         <v>4495</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="19">
         <v>7850</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
       <c r="H16" s="15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I16" s="17">
-        <v>4495</v>
-      </c>
-      <c r="J16" s="32">
-        <v>7850</v>
-      </c>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
+        <v>5287</v>
+      </c>
+      <c r="J16" s="40">
+        <v>113620</v>
+      </c>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
     </row>
     <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
@@ -1109,22 +1106,16 @@
       <c r="B17" s="1">
         <v>4498</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="18">
         <v>1348</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="H17" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" s="17">
-        <v>4498</v>
-      </c>
-      <c r="J17" s="32">
-        <v>1348</v>
-      </c>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
     </row>
     <row r="18" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -1133,107 +1124,107 @@
       <c r="B18" s="2">
         <v>4603</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="19">
         <v>1348</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
       <c r="H18" s="15"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
     </row>
     <row r="19" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
       <c r="H19" s="15"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
     </row>
     <row r="20" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
       <c r="H20" s="15"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
     </row>
     <row r="21" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
       <c r="H21" s="3"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
     </row>
     <row r="22" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
       <c r="H22" s="6"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
     </row>
     <row r="23" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="42">
+      <c r="B23" s="24"/>
+      <c r="C23" s="21">
         <f>SUM(C15:C22)</f>
         <v>11220</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I23" s="21"/>
+      <c r="I23" s="24"/>
       <c r="J23" s="22">
         <f>SUM(J15:J22)</f>
-        <v>129135</v>
+        <v>114968</v>
       </c>
       <c r="K23" s="22"/>
       <c r="L23" s="22"/>
     </row>
     <row r="25" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="27" t="s">
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="28"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="4"/>
-      <c r="H25" s="24" t="s">
+      <c r="H25" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="25"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="27">
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="30">
         <v>45696</v>
       </c>
-      <c r="L25" s="28"/>
+      <c r="L25" s="29"/>
     </row>
     <row r="26" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
@@ -1242,22 +1233,22 @@
       <c r="B26" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="36"/>
-      <c r="E26" s="37"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="33"/>
       <c r="H26" s="13" t="s">
         <v>12</v>
       </c>
       <c r="I26" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J26" s="29" t="s">
+      <c r="J26" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="K26" s="30"/>
-      <c r="L26" s="31"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="39"/>
     </row>
     <row r="27" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
@@ -1266,22 +1257,22 @@
       <c r="B27" s="1">
         <v>5100</v>
       </c>
-      <c r="C27" s="23">
+      <c r="C27" s="18">
         <v>37164</v>
       </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
       <c r="H27" s="15" t="s">
         <v>13</v>
       </c>
       <c r="I27" s="16">
         <v>4509</v>
       </c>
-      <c r="J27" s="32">
+      <c r="J27" s="40">
         <v>74081</v>
       </c>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
     </row>
     <row r="28" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
@@ -1290,110 +1281,110 @@
       <c r="B28" s="2">
         <v>4898</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28" s="19">
         <v>129347</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
       <c r="H28" s="15" t="s">
         <v>14</v>
       </c>
       <c r="I28" s="17">
         <v>4296</v>
       </c>
-      <c r="J28" s="33">
+      <c r="J28" s="41">
         <v>785</v>
       </c>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
     </row>
     <row r="29" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
       <c r="H29" s="3"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
     </row>
     <row r="30" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
       <c r="H30" s="3"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
     </row>
     <row r="31" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
       <c r="H31" s="3"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
     </row>
     <row r="32" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
       <c r="H32" s="3"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
     </row>
     <row r="33" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
       <c r="H33" s="3"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
     </row>
     <row r="34" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
       <c r="H34" s="6"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
     </row>
     <row r="35" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="42">
+      <c r="B35" s="24"/>
+      <c r="C35" s="21">
         <f>SUM(C27:C34)</f>
         <v>166511</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
-      <c r="H35" s="20" t="s">
+      <c r="H35" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I35" s="21"/>
+      <c r="I35" s="24"/>
       <c r="J35" s="22">
         <f>SUM(J27:J34)</f>
         <v>74866</v>
@@ -1403,6 +1394,68 @@
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E35"/>
@@ -1419,68 +1472,6 @@
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C32:E32"/>
     <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:L35"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="J33:L33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>